<commit_message>
Working cheker if the balance is off
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/xlsx_files/Booking-report-125295-Own.Solutions---Tobaccoland-API-08-2024-tobaccoland.xlsx
+++ b/src/main/java/org/example/xlsx_files/Booking-report-125295-Own.Solutions---Tobaccoland-API-08-2024-tobaccoland.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anavolaric/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\OneDrive\Documents\GitHub\DifferenceFinder\src\main\java\org\example\xlsx_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C9008-B799-0C45-AEC6-C44E1ED46154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3028459E-CA8B-4985-B992-C5E1BE06ABA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1781,32 +1781,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S3348"/>
+  <dimension ref="A1:S516"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P528" sqref="P528"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="37.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="6" width="90.83203125" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" customWidth="1"/>
-    <col min="9" max="9" width="23.83203125" customWidth="1"/>
-    <col min="10" max="10" width="45.83203125" customWidth="1"/>
-    <col min="11" max="11" width="76.83203125" customWidth="1"/>
-    <col min="12" max="12" width="23.83203125" customWidth="1"/>
-    <col min="13" max="15" width="10.83203125" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" customWidth="1"/>
-    <col min="18" max="19" width="11.83203125" customWidth="1"/>
+    <col min="1" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="90.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" customWidth="1"/>
+    <col min="11" max="11" width="76.85546875" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" customWidth="1"/>
+    <col min="13" max="15" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="19" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>125295</v>
       </c>
       <c r="D3">
-        <v>3182868480</v>
+        <v>3100000000</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -1983,7 +1983,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>14.87</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>28.82</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>6.97</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>39.049999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>38.119999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>38.119999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>60</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>60</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -4402,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>125295</v>
       </c>
       <c r="D63">
-        <v>3181740676</v>
+        <v>3000000000</v>
       </c>
       <c r="E63" t="s">
         <v>34</v>
@@ -5523,7 +5523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>60</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -5818,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>60</v>
       </c>
@@ -5936,7 +5936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>60</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>60</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>56</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>56</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>38.119999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>56</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>56</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>16.739999999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>56</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>14.88</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>56</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>56</v>
       </c>
@@ -6762,7 +6762,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>56</v>
       </c>
@@ -6821,7 +6821,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>56</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>92.06</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>56</v>
       </c>
@@ -6939,7 +6939,7 @@
         <v>51.14</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>56</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>56</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>100.43</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>56</v>
       </c>
@@ -7116,7 +7116,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>56</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>56</v>
       </c>
@@ -7234,7 +7234,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>56</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>56</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>56</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>56</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>84.62</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>56</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>56</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>67.88</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>56</v>
       </c>
@@ -7647,7 +7647,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>56</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>56</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>56</v>
       </c>
@@ -7824,7 +7824,7 @@
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>56</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>56</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>56</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>56</v>
       </c>
@@ -8060,7 +8060,7 @@
         <v>48.35</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>56</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>63.23</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>56</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>56</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>56</v>
       </c>
@@ -8296,7 +8296,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>56</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>56</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="113" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>56</v>
       </c>
@@ -8473,7 +8473,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="114" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>56</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="115" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>56</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="116" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>56</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>14.87</v>
       </c>
     </row>
-    <row r="117" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>56</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>11.62</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>56</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="119" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>56</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>56</v>
       </c>
@@ -8886,7 +8886,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="121" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>56</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>56</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="123" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -9063,7 +9063,7 @@
         <v>19.989999999999998</v>
       </c>
     </row>
-    <row r="124" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>56</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="125" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>56</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="126" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>56</v>
       </c>
@@ -9240,7 +9240,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="127" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>56</v>
       </c>
@@ -9299,7 +9299,7 @@
         <v>24.17</v>
       </c>
     </row>
-    <row r="128" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>56</v>
       </c>
@@ -9358,7 +9358,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>56</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>56</v>
       </c>
@@ -9476,7 +9476,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>56</v>
       </c>
@@ -9535,7 +9535,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>56</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>8.36</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>56</v>
       </c>
@@ -9653,7 +9653,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>56</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>64.16</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>56</v>
       </c>
@@ -9771,7 +9771,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>56</v>
       </c>
@@ -9830,7 +9830,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -9889,7 +9889,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>56</v>
       </c>
@@ -9948,7 +9948,7 @@
         <v>21.38</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>56</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>21.38</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>56</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>21.38</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>56</v>
       </c>
@@ -10125,7 +10125,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>56</v>
       </c>
@@ -10184,7 +10184,7 @@
         <v>53.93</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>56</v>
       </c>
@@ -10243,7 +10243,7 @@
         <v>73.459999999999994</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>56</v>
       </c>
@@ -10302,7 +10302,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>56</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>112.52</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>56</v>
       </c>
@@ -10420,7 +10420,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>56</v>
       </c>
@@ -10479,7 +10479,7 @@
         <v>59.51</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>56</v>
       </c>
@@ -10538,7 +10538,7 @@
         <v>59.51</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>56</v>
       </c>
@@ -10597,7 +10597,7 @@
         <v>59.51</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>56</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>56</v>
       </c>
@@ -10715,7 +10715,7 @@
         <v>42.77</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>56</v>
       </c>
@@ -10774,7 +10774,7 @@
         <v>46.49</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>56</v>
       </c>
@@ -10833,7 +10833,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>56</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>56</v>
       </c>
@@ -10951,7 +10951,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>56</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>56</v>
       </c>
@@ -11069,7 +11069,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>56</v>
       </c>
@@ -11128,7 +11128,7 @@
         <v>23.71</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>56</v>
       </c>
@@ -11187,7 +11187,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>56</v>
       </c>
@@ -11246,7 +11246,7 @@
         <v>14.41</v>
       </c>
     </row>
-    <row r="161" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>56</v>
       </c>
@@ -11305,7 +11305,7 @@
         <v>13.01</v>
       </c>
     </row>
-    <row r="162" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>9</v>
       </c>
@@ -11364,7 +11364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>9</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -11482,7 +11482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -11541,7 +11541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>9</v>
       </c>
@@ -11600,7 +11600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>9</v>
       </c>
@@ -11659,7 +11659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>9</v>
       </c>
@@ -11718,7 +11718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>56</v>
       </c>
@@ -11777,7 +11777,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="170" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>56</v>
       </c>
@@ -11836,7 +11836,7 @@
         <v>22.31</v>
       </c>
     </row>
-    <row r="171" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>56</v>
       </c>
@@ -11895,7 +11895,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="172" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>56</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>20.92</v>
       </c>
     </row>
-    <row r="173" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>56</v>
       </c>
@@ -12013,7 +12013,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="174" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>56</v>
       </c>
@@ -12072,7 +12072,7 @@
         <v>68.81</v>
       </c>
     </row>
-    <row r="175" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>56</v>
       </c>
@@ -12131,7 +12131,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="176" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>56</v>
       </c>
@@ -12190,7 +12190,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>56</v>
       </c>
@@ -12249,7 +12249,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>56</v>
       </c>
@@ -12308,7 +12308,7 @@
         <v>45.56</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>56</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>51.14</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>56</v>
       </c>
@@ -12426,7 +12426,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>56</v>
       </c>
@@ -12485,7 +12485,7 @@
         <v>32.54</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>56</v>
       </c>
@@ -12544,7 +12544,7 @@
         <v>32.54</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>9</v>
       </c>
@@ -12603,7 +12603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>9</v>
       </c>
@@ -12662,7 +12662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>9</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>9</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>9</v>
       </c>
@@ -12898,7 +12898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>9</v>
       </c>
@@ -12957,7 +12957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>9</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>56</v>
       </c>
@@ -13075,7 +13075,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>56</v>
       </c>
@@ -13134,7 +13134,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="193" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>56</v>
       </c>
@@ -13193,7 +13193,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="194" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>56</v>
       </c>
@@ -13252,7 +13252,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="195" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>56</v>
       </c>
@@ -13311,7 +13311,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="196" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>56</v>
       </c>
@@ -13370,7 +13370,7 @@
         <v>121.82</v>
       </c>
     </row>
-    <row r="197" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>56</v>
       </c>
@@ -13429,7 +13429,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="198" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>56</v>
       </c>
@@ -13488,7 +13488,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="199" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>60</v>
       </c>
@@ -13547,7 +13547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>60</v>
       </c>
@@ -13606,7 +13606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>60</v>
       </c>
@@ -13665,7 +13665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>60</v>
       </c>
@@ -13724,7 +13724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>60</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>60</v>
       </c>
@@ -13842,7 +13842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>60</v>
       </c>
@@ -13901,7 +13901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>60</v>
       </c>
@@ -13960,7 +13960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>56</v>
       </c>
@@ -14019,7 +14019,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="208" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>56</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>26.04</v>
       </c>
     </row>
-    <row r="209" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>56</v>
       </c>
@@ -14137,7 +14137,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="210" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>56</v>
       </c>
@@ -14196,7 +14196,7 @@
         <v>20.92</v>
       </c>
     </row>
-    <row r="211" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>56</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="212" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>56</v>
       </c>
@@ -14314,7 +14314,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="213" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>60</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>60</v>
       </c>
@@ -14432,7 +14432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>60</v>
       </c>
@@ -14491,7 +14491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>60</v>
       </c>
@@ -14550,7 +14550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>56</v>
       </c>
@@ -14609,7 +14609,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="218" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>56</v>
       </c>
@@ -14668,7 +14668,7 @@
         <v>17.66</v>
       </c>
     </row>
-    <row r="219" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>56</v>
       </c>
@@ -14727,7 +14727,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="220" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>56</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="221" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>56</v>
       </c>
@@ -14845,7 +14845,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="222" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>56</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="223" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>56</v>
       </c>
@@ -14963,7 +14963,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="224" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>56</v>
       </c>
@@ -15022,7 +15022,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="225" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>56</v>
       </c>
@@ -15081,7 +15081,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="226" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>56</v>
       </c>
@@ -15140,7 +15140,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="227" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>56</v>
       </c>
@@ -15199,7 +15199,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="228" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>56</v>
       </c>
@@ -15258,7 +15258,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="229" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>56</v>
       </c>
@@ -15317,7 +15317,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="230" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>56</v>
       </c>
@@ -15376,7 +15376,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="231" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>56</v>
       </c>
@@ -15435,7 +15435,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="232" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>56</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="233" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>56</v>
       </c>
@@ -15553,7 +15553,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="234" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>56</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="235" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>56</v>
       </c>
@@ -15671,7 +15671,7 @@
         <v>79.040000000000006</v>
       </c>
     </row>
-    <row r="236" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>56</v>
       </c>
@@ -15730,7 +15730,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="237" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>56</v>
       </c>
@@ -15789,7 +15789,7 @@
         <v>33.47</v>
       </c>
     </row>
-    <row r="238" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>56</v>
       </c>
@@ -15848,7 +15848,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="239" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>56</v>
       </c>
@@ -15907,7 +15907,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="240" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>56</v>
       </c>
@@ -15966,7 +15966,7 @@
         <v>46.49</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>56</v>
       </c>
@@ -16025,7 +16025,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>56</v>
       </c>
@@ -16084,7 +16084,7 @@
         <v>79.040000000000006</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>56</v>
       </c>
@@ -16143,7 +16143,7 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>56</v>
       </c>
@@ -16202,7 +16202,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>56</v>
       </c>
@@ -16261,7 +16261,7 @@
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>56</v>
       </c>
@@ -16320,7 +16320,7 @@
         <v>30.69</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>56</v>
       </c>
@@ -16379,7 +16379,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>56</v>
       </c>
@@ -16438,7 +16438,7 @@
         <v>42.77</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>56</v>
       </c>
@@ -16497,7 +16497,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>56</v>
       </c>
@@ -16556,7 +16556,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>56</v>
       </c>
@@ -16615,7 +16615,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>56</v>
       </c>
@@ -16674,7 +16674,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="253" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>56</v>
       </c>
@@ -16733,7 +16733,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="254" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>56</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="255" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>56</v>
       </c>
@@ -16851,7 +16851,7 @@
         <v>12.56</v>
       </c>
     </row>
-    <row r="256" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>56</v>
       </c>
@@ -16910,7 +16910,7 @@
         <v>12.56</v>
       </c>
     </row>
-    <row r="257" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>56</v>
       </c>
@@ -16969,7 +16969,7 @@
         <v>12.56</v>
       </c>
     </row>
-    <row r="258" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>56</v>
       </c>
@@ -17028,7 +17028,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="259" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>56</v>
       </c>
@@ -17087,7 +17087,7 @@
         <v>52.07</v>
       </c>
     </row>
-    <row r="260" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>56</v>
       </c>
@@ -17146,7 +17146,7 @@
         <v>70.67</v>
       </c>
     </row>
-    <row r="261" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>56</v>
       </c>
@@ -17205,7 +17205,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="262" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>56</v>
       </c>
@@ -17264,7 +17264,7 @@
         <v>66.95</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>60</v>
       </c>
@@ -17323,7 +17323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>60</v>
       </c>
@@ -17382,7 +17382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>60</v>
       </c>
@@ -17441,7 +17441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>60</v>
       </c>
@@ -17500,7 +17500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>60</v>
       </c>
@@ -17559,7 +17559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>60</v>
       </c>
@@ -17618,7 +17618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>60</v>
       </c>
@@ -17677,7 +17677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>60</v>
       </c>
@@ -17736,7 +17736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>60</v>
       </c>
@@ -17795,7 +17795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>60</v>
       </c>
@@ -17854,7 +17854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>60</v>
       </c>
@@ -17913,7 +17913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>60</v>
       </c>
@@ -17972,7 +17972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>60</v>
       </c>
@@ -18031,7 +18031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>60</v>
       </c>
@@ -18090,7 +18090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>60</v>
       </c>
@@ -18149,7 +18149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>60</v>
       </c>
@@ -18208,7 +18208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>60</v>
       </c>
@@ -18267,7 +18267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>60</v>
       </c>
@@ -18326,7 +18326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>56</v>
       </c>
@@ -18385,7 +18385,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="282" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>56</v>
       </c>
@@ -18444,7 +18444,7 @@
         <v>17.66</v>
       </c>
     </row>
-    <row r="283" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>56</v>
       </c>
@@ -18503,7 +18503,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="284" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>56</v>
       </c>
@@ -18562,7 +18562,7 @@
         <v>22.78</v>
       </c>
     </row>
-    <row r="285" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>56</v>
       </c>
@@ -18621,7 +18621,7 @@
         <v>22.78</v>
       </c>
     </row>
-    <row r="286" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>56</v>
       </c>
@@ -18680,7 +18680,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="287" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>56</v>
       </c>
@@ -18739,7 +18739,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="288" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>56</v>
       </c>
@@ -18798,7 +18798,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="289" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>56</v>
       </c>
@@ -18857,7 +18857,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="290" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>56</v>
       </c>
@@ -18916,7 +18916,7 @@
         <v>21.38</v>
       </c>
     </row>
-    <row r="291" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>56</v>
       </c>
@@ -18975,7 +18975,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="292" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>56</v>
       </c>
@@ -19034,7 +19034,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="293" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>56</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="294" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>56</v>
       </c>
@@ -19152,7 +19152,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="295" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>56</v>
       </c>
@@ -19211,7 +19211,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="296" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>56</v>
       </c>
@@ -19270,7 +19270,7 @@
         <v>24.18</v>
       </c>
     </row>
-    <row r="297" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>56</v>
       </c>
@@ -19329,7 +19329,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="298" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>56</v>
       </c>
@@ -19388,7 +19388,7 @@
         <v>24.18</v>
       </c>
     </row>
-    <row r="299" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>56</v>
       </c>
@@ -19447,7 +19447,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="300" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>56</v>
       </c>
@@ -19506,7 +19506,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="301" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>56</v>
       </c>
@@ -19565,7 +19565,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="302" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>56</v>
       </c>
@@ -19624,7 +19624,7 @@
         <v>13.02</v>
       </c>
     </row>
-    <row r="303" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>56</v>
       </c>
@@ -19683,7 +19683,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="304" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>56</v>
       </c>
@@ -19742,7 +19742,7 @@
         <v>89.27</v>
       </c>
     </row>
-    <row r="305" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>56</v>
       </c>
@@ -19801,7 +19801,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="306" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>56</v>
       </c>
@@ -19860,7 +19860,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="307" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>56</v>
       </c>
@@ -19919,7 +19919,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="308" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>56</v>
       </c>
@@ -19978,7 +19978,7 @@
         <v>35.33</v>
       </c>
     </row>
-    <row r="309" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>56</v>
       </c>
@@ -20037,7 +20037,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="310" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>56</v>
       </c>
@@ -20096,7 +20096,7 @@
         <v>28.82</v>
       </c>
     </row>
-    <row r="311" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>56</v>
       </c>
@@ -20155,7 +20155,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="312" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>56</v>
       </c>
@@ -20214,7 +20214,7 @@
         <v>47.42</v>
       </c>
     </row>
-    <row r="313" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>56</v>
       </c>
@@ -20273,7 +20273,7 @@
         <v>14.41</v>
       </c>
     </row>
-    <row r="314" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>56</v>
       </c>
@@ -20332,7 +20332,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="315" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>56</v>
       </c>
@@ -20391,7 +20391,7 @@
         <v>16.739999999999998</v>
       </c>
     </row>
-    <row r="316" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>56</v>
       </c>
@@ -20450,7 +20450,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="317" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>56</v>
       </c>
@@ -20509,7 +20509,7 @@
         <v>95.78</v>
       </c>
     </row>
-    <row r="318" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>60</v>
       </c>
@@ -20568,7 +20568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>60</v>
       </c>
@@ -20627,7 +20627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>60</v>
       </c>
@@ -20686,7 +20686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>60</v>
       </c>
@@ -20745,7 +20745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>9</v>
       </c>
@@ -20804,7 +20804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>9</v>
       </c>
@@ -20863,7 +20863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>9</v>
       </c>
@@ -20922,7 +20922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>9</v>
       </c>
@@ -20981,7 +20981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>56</v>
       </c>
@@ -21040,7 +21040,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="327" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>56</v>
       </c>
@@ -21099,7 +21099,7 @@
         <v>23.24</v>
       </c>
     </row>
-    <row r="328" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>9</v>
       </c>
@@ -21158,7 +21158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>9</v>
       </c>
@@ -21217,7 +21217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>9</v>
       </c>
@@ -21276,7 +21276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>9</v>
       </c>
@@ -21335,7 +21335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>9</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>9</v>
       </c>
@@ -21453,7 +21453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>9</v>
       </c>
@@ -21512,7 +21512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>9</v>
       </c>
@@ -21571,7 +21571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>56</v>
       </c>
@@ -21630,7 +21630,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="337" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>56</v>
       </c>
@@ -21689,7 +21689,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="338" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>56</v>
       </c>
@@ -21748,7 +21748,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="339" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>56</v>
       </c>
@@ -21807,7 +21807,7 @@
         <v>61.37</v>
       </c>
     </row>
-    <row r="340" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>56</v>
       </c>
@@ -21866,7 +21866,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="341" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>56</v>
       </c>
@@ -21925,7 +21925,7 @@
         <v>30.68</v>
       </c>
     </row>
-    <row r="342" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>56</v>
       </c>
@@ -21984,7 +21984,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="343" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>56</v>
       </c>
@@ -22043,7 +22043,7 @@
         <v>30.69</v>
       </c>
     </row>
-    <row r="344" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>56</v>
       </c>
@@ -22102,7 +22102,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="345" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>56</v>
       </c>
@@ -22161,7 +22161,7 @@
         <v>16.739999999999998</v>
       </c>
     </row>
-    <row r="346" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>56</v>
       </c>
@@ -22220,7 +22220,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="347" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>56</v>
       </c>
@@ -22279,7 +22279,7 @@
         <v>16.739999999999998</v>
       </c>
     </row>
-    <row r="348" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>56</v>
       </c>
@@ -22338,7 +22338,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="349" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>56</v>
       </c>
@@ -22397,7 +22397,7 @@
         <v>74.39</v>
       </c>
     </row>
-    <row r="350" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>56</v>
       </c>
@@ -22456,7 +22456,7 @@
         <v>74.39</v>
       </c>
     </row>
-    <row r="351" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>56</v>
       </c>
@@ -22515,7 +22515,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="352" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>56</v>
       </c>
@@ -22574,7 +22574,7 @@
         <v>43.7</v>
       </c>
     </row>
-    <row r="353" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>56</v>
       </c>
@@ -22633,7 +22633,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="354" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>56</v>
       </c>
@@ -22692,7 +22692,7 @@
         <v>27.89</v>
       </c>
     </row>
-    <row r="355" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>56</v>
       </c>
@@ -22751,7 +22751,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="356" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>56</v>
       </c>
@@ -22810,7 +22810,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="357" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>56</v>
       </c>
@@ -22869,7 +22869,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="358" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>56</v>
       </c>
@@ -22928,7 +22928,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="359" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>56</v>
       </c>
@@ -22987,7 +22987,7 @@
         <v>27.89</v>
       </c>
     </row>
-    <row r="360" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>56</v>
       </c>
@@ -23046,7 +23046,7 @@
         <v>37.19</v>
       </c>
     </row>
-    <row r="361" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>9</v>
       </c>
@@ -23105,7 +23105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>9</v>
       </c>
@@ -23164,7 +23164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>9</v>
       </c>
@@ -23223,7 +23223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>9</v>
       </c>
@@ -23282,7 +23282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>9</v>
       </c>
@@ -23341,7 +23341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>56</v>
       </c>
@@ -23400,7 +23400,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="367" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>56</v>
       </c>
@@ -23459,7 +23459,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="368" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>56</v>
       </c>
@@ -23518,7 +23518,7 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="369" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>56</v>
       </c>
@@ -23577,7 +23577,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="370" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>56</v>
       </c>
@@ -23636,7 +23636,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="371" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>60</v>
       </c>
@@ -23695,7 +23695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>60</v>
       </c>
@@ -23754,7 +23754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>60</v>
       </c>
@@ -23813,7 +23813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>60</v>
       </c>
@@ -23872,7 +23872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>56</v>
       </c>
@@ -23931,7 +23931,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="376" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>56</v>
       </c>
@@ -23990,7 +23990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="377" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>56</v>
       </c>
@@ -24049,7 +24049,7 @@
         <v>92.99</v>
       </c>
     </row>
-    <row r="378" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>56</v>
       </c>
@@ -24108,7 +24108,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="379" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>56</v>
       </c>
@@ -24167,7 +24167,7 @@
         <v>49.28</v>
       </c>
     </row>
-    <row r="380" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>56</v>
       </c>
@@ -24226,7 +24226,7 @@
         <v>41.85</v>
       </c>
     </row>
-    <row r="381" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>56</v>
       </c>
@@ -24285,7 +24285,7 @@
         <v>-0.99</v>
       </c>
     </row>
-    <row r="382" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>56</v>
       </c>
@@ -24344,7 +24344,7 @@
         <v>-49.28</v>
       </c>
     </row>
-    <row r="383" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>56</v>
       </c>
@@ -24403,7 +24403,7 @@
         <v>-41.85</v>
       </c>
     </row>
-    <row r="384" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>56</v>
       </c>
@@ -24462,7 +24462,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="385" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>56</v>
       </c>
@@ -24521,7 +24521,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="386" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>56</v>
       </c>
@@ -24580,7 +24580,7 @@
         <v>31.61</v>
       </c>
     </row>
-    <row r="387" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>60</v>
       </c>
@@ -24639,7 +24639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>60</v>
       </c>
@@ -24698,7 +24698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>60</v>
       </c>
@@ -24757,7 +24757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>60</v>
       </c>
@@ -24816,7 +24816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>60</v>
       </c>
@@ -24875,7 +24875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>60</v>
       </c>
@@ -24934,7 +24934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>60</v>
       </c>
@@ -24993,7 +24993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>60</v>
       </c>
@@ -25052,7 +25052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>60</v>
       </c>
@@ -25111,7 +25111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>60</v>
       </c>
@@ -25170,7 +25170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>60</v>
       </c>
@@ -25229,7 +25229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>60</v>
       </c>
@@ -25288,7 +25288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>60</v>
       </c>
@@ -25347,7 +25347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>60</v>
       </c>
@@ -25406,7 +25406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>60</v>
       </c>
@@ -25465,7 +25465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>60</v>
       </c>
@@ -25524,7 +25524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>60</v>
       </c>
@@ -25583,7 +25583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>60</v>
       </c>
@@ -25642,7 +25642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>60</v>
       </c>
@@ -25701,7 +25701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>60</v>
       </c>
@@ -25760,7 +25760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>60</v>
       </c>
@@ -25819,7 +25819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>60</v>
       </c>
@@ -25878,7 +25878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>60</v>
       </c>
@@ -25937,7 +25937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>60</v>
       </c>
@@ -25996,7 +25996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>60</v>
       </c>
@@ -26055,7 +26055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>60</v>
       </c>
@@ -26114,7 +26114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>60</v>
       </c>
@@ -26173,7 +26173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>60</v>
       </c>
@@ -26232,7 +26232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>60</v>
       </c>
@@ -26291,7 +26291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>60</v>
       </c>
@@ -26350,7 +26350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>60</v>
       </c>
@@ -26409,7 +26409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>60</v>
       </c>
@@ -26468,7 +26468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>60</v>
       </c>
@@ -26527,7 +26527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>60</v>
       </c>
@@ -26586,7 +26586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>60</v>
       </c>
@@ -26645,7 +26645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>60</v>
       </c>
@@ -26704,7 +26704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>60</v>
       </c>
@@ -26763,7 +26763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>60</v>
       </c>
@@ -26822,7 +26822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>60</v>
       </c>
@@ -26881,7 +26881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>60</v>
       </c>
@@ -26940,7 +26940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>60</v>
       </c>
@@ -26999,7 +26999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>60</v>
       </c>
@@ -27058,7 +27058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>56</v>
       </c>
@@ -27117,7 +27117,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="430" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>56</v>
       </c>
@@ -27176,7 +27176,7 @@
         <v>31.61</v>
       </c>
     </row>
-    <row r="431" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>56</v>
       </c>
@@ -27235,7 +27235,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="432" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>56</v>
       </c>
@@ -27294,7 +27294,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="433" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>56</v>
       </c>
@@ -27353,7 +27353,7 @@
         <v>78.11</v>
       </c>
     </row>
-    <row r="434" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>56</v>
       </c>
@@ -27412,7 +27412,7 @@
         <v>52.07</v>
       </c>
     </row>
-    <row r="435" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>56</v>
       </c>
@@ -27471,7 +27471,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="436" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>56</v>
       </c>
@@ -27530,7 +27530,7 @@
         <v>25.11</v>
       </c>
     </row>
-    <row r="437" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>60</v>
       </c>
@@ -27589,7 +27589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>60</v>
       </c>
@@ -27648,7 +27648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>60</v>
       </c>
@@ -27707,7 +27707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>60</v>
       </c>
@@ -27766,7 +27766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>60</v>
       </c>
@@ -27825,7 +27825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>60</v>
       </c>
@@ -27884,7 +27884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>56</v>
       </c>
@@ -27943,7 +27943,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="444" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>56</v>
       </c>
@@ -28002,7 +28002,7 @@
         <v>28.82</v>
       </c>
     </row>
-    <row r="445" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>56</v>
       </c>
@@ -28061,7 +28061,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="446" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>56</v>
       </c>
@@ -28120,7 +28120,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="447" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>56</v>
       </c>
@@ -28179,7 +28179,7 @@
         <v>32.54</v>
       </c>
     </row>
-    <row r="448" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>60</v>
       </c>
@@ -28238,7 +28238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>60</v>
       </c>
@@ -28297,7 +28297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>60</v>
       </c>
@@ -28356,7 +28356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>60</v>
       </c>
@@ -28415,7 +28415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>60</v>
       </c>
@@ -28474,7 +28474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>60</v>
       </c>
@@ -28533,7 +28533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>60</v>
       </c>
@@ -28592,7 +28592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>60</v>
       </c>
@@ -28651,7 +28651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>60</v>
       </c>
@@ -28710,7 +28710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>60</v>
       </c>
@@ -28769,7 +28769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>60</v>
       </c>
@@ -28828,7 +28828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>60</v>
       </c>
@@ -28887,7 +28887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>60</v>
       </c>
@@ -28946,7 +28946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>60</v>
       </c>
@@ -29005,7 +29005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>60</v>
       </c>
@@ -29064,7 +29064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>60</v>
       </c>
@@ -29123,7 +29123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>60</v>
       </c>
@@ -29182,7 +29182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>60</v>
       </c>
@@ -29241,7 +29241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>56</v>
       </c>
@@ -29300,7 +29300,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="467" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>56</v>
       </c>
@@ -29359,7 +29359,7 @@
         <v>49.28</v>
       </c>
     </row>
-    <row r="468" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>56</v>
       </c>
@@ -29418,7 +29418,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="469" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>56</v>
       </c>
@@ -29477,7 +29477,7 @@
         <v>19.059999999999999</v>
       </c>
     </row>
-    <row r="470" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>56</v>
       </c>
@@ -29536,7 +29536,7 @@
         <v>27.89</v>
       </c>
     </row>
-    <row r="471" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>56</v>
       </c>
@@ -29595,7 +29595,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="472" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>56</v>
       </c>
@@ -29654,7 +29654,7 @@
         <v>27.89</v>
       </c>
     </row>
-    <row r="473" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>56</v>
       </c>
@@ -29713,7 +29713,7 @@
         <v>26.03</v>
       </c>
     </row>
-    <row r="474" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>56</v>
       </c>
@@ -29772,7 +29772,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="475" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>56</v>
       </c>
@@ -29831,7 +29831,7 @@
         <v>41.84</v>
       </c>
     </row>
-    <row r="476" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>56</v>
       </c>
@@ -29890,7 +29890,7 @@
         <v>43.7</v>
       </c>
     </row>
-    <row r="477" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>56</v>
       </c>
@@ -29949,7 +29949,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="478" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>56</v>
       </c>
@@ -30008,7 +30008,7 @@
         <v>30.68</v>
       </c>
     </row>
-    <row r="479" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>56</v>
       </c>
@@ -30067,7 +30067,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="480" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>56</v>
       </c>
@@ -30126,7 +30126,7 @@
         <v>36.26</v>
       </c>
     </row>
-    <row r="481" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>56</v>
       </c>
@@ -30185,7 +30185,7 @@
         <v>35.57</v>
       </c>
     </row>
-    <row r="482" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>56</v>
       </c>
@@ -30244,7 +30244,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="483" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>56</v>
       </c>
@@ -30303,7 +30303,7 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="484" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>56</v>
       </c>
@@ -30362,7 +30362,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="485" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>56</v>
       </c>
@@ -30421,7 +30421,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="486" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>56</v>
       </c>
@@ -30480,7 +30480,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="487" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>56</v>
       </c>
@@ -30539,7 +30539,7 @@
         <v>6.97</v>
       </c>
     </row>
-    <row r="488" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>56</v>
       </c>
@@ -30598,7 +30598,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="489" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>56</v>
       </c>
@@ -30657,7 +30657,7 @@
         <v>66.95</v>
       </c>
     </row>
-    <row r="490" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>56</v>
       </c>
@@ -30716,7 +30716,7 @@
         <v>56.72</v>
       </c>
     </row>
-    <row r="491" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>56</v>
       </c>
@@ -30775,7 +30775,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="492" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>56</v>
       </c>
@@ -30834,7 +30834,7 @@
         <v>66.95</v>
       </c>
     </row>
-    <row r="493" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>56</v>
       </c>
@@ -30893,7 +30893,7 @@
         <v>56.72</v>
       </c>
     </row>
-    <row r="494" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>60</v>
       </c>
@@ -30952,7 +30952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>60</v>
       </c>
@@ -31011,7 +31011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>60</v>
       </c>
@@ -31070,7 +31070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>60</v>
       </c>
@@ -31129,7 +31129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>60</v>
       </c>
@@ -31188,7 +31188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>60</v>
       </c>
@@ -31247,7 +31247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>60</v>
       </c>
@@ -31306,7 +31306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>60</v>
       </c>
@@ -31365,7 +31365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>60</v>
       </c>
@@ -31424,7 +31424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>60</v>
       </c>
@@ -31483,7 +31483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>60</v>
       </c>
@@ -31542,7 +31542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="505" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>60</v>
       </c>
@@ -31601,7 +31601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>56</v>
       </c>
@@ -31660,7 +31660,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="507" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>56</v>
       </c>
@@ -31719,7 +31719,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="508" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>56</v>
       </c>
@@ -31778,7 +31778,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="509" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>56</v>
       </c>
@@ -31837,7 +31837,7 @@
         <v>74.39</v>
       </c>
     </row>
-    <row r="510" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>56</v>
       </c>
@@ -31896,7 +31896,7 @@
         <v>70.67</v>
       </c>
     </row>
-    <row r="511" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>56</v>
       </c>
@@ -31955,7 +31955,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="512" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>56</v>
       </c>
@@ -32014,7 +32014,7 @@
         <v>46.49</v>
       </c>
     </row>
-    <row r="513" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>56</v>
       </c>
@@ -32073,7 +32073,7 @@
         <v>32.54</v>
       </c>
     </row>
-    <row r="514" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>56</v>
       </c>
@@ -32132,7 +32132,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="515" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>56</v>
       </c>
@@ -32191,7 +32191,7 @@
         <v>21.39</v>
       </c>
     </row>
-    <row r="516" spans="1:19" ht="15" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A516" s="1" t="s">
         <v>452</v>
       </c>
@@ -32248,13 +32248,10 @@
         <v>6310.0999999999822</v>
       </c>
     </row>
-    <row r="517" spans="1:19" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="3347" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="3348" ht="15" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:S1 A2:S515 A516:M516" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:S1 A2:S2 A516:M516 A64:S515 A63:C63 E63:S63 A18:S62 A17:C17 E17:S17 A4:S16 A3:C3 E3:S3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>